<commit_message>
update steel indicators plot to deal with changed indicator names in Wind
</commit_message>
<xml_diff>
--- a/data/label_translations.xlsx
+++ b/data/label_translations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="306">
   <si>
     <t>EN</t>
   </si>
@@ -662,6 +662,9 @@
   </si>
   <si>
     <t>线材：主要钢厂开工率</t>
+  </si>
+  <si>
+    <t>Operating Rate: Wire Rod</t>
   </si>
   <si>
     <t>Source: Wind Information</t>
@@ -2117,100 +2120,100 @@
         <v>217</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>23</v>
+        <v>231</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>231</v>
+        <v>23</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>232</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>15</v>
@@ -2221,7 +2224,7 @@
         <v>234</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
     </row>
     <row r="129">
@@ -2229,39 +2232,39 @@
         <v>235</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>96</v>
+        <v>236</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>228</v>
+        <v>101</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>236</v>
+        <v>96</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>99</v>
+        <v>240</v>
       </c>
     </row>
     <row r="134">
@@ -2269,28 +2272,28 @@
         <v>235</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>241</v>
+        <v>101</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>244</v>
@@ -2298,18 +2301,18 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="140">
@@ -2317,79 +2320,79 @@
         <v>248</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B142" s="1" t="s">
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="2" t="s">
+      <c r="B143" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B143" s="2" t="s">
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="s">
+      <c r="B144" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B145" s="2" t="s">
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B146" s="2" t="s">
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="s">
+      <c r="B147" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="150">
@@ -2397,52 +2400,52 @@
         <v>267</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>269</v>
+      <c r="B151" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>278</v>
@@ -2450,26 +2453,26 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="160">
@@ -2477,28 +2480,28 @@
         <v>284</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>285</v>
+        <v>162</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>173</v>
+        <v>289</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>290</v>
@@ -2506,58 +2509,66 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B170" s="1" t="s">
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="s">
         <v>304</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>